<commit_message>
Implemented rendering of single student results page per session and term. created a view for merging first and second term results to third term for display.
</commit_message>
<xml_diff>
--- a/SchoolPortal.Web/wwwroot/templates/Batch Upload End-Term Results Template.xlsx
+++ b/SchoolPortal.Web/wwwroot/templates/Batch Upload End-Term Results Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariofrancis\source\repos\SchoolPortal\SchoolPortal.Web\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CD619E-6C15-49FD-9B92-D673035BE8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2ED9AA-A2F2-44F7-9808-105851BABF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="1815" windowWidth="19995" windowHeight="13125" xr2:uid="{D4E0B7BB-266D-4FFE-864F-F1915E4699E5}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +480,10 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -500,10 +500,10 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F3" s="5">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>